<commit_message>
Refactor export to excel func
</commit_message>
<xml_diff>
--- a/edge_research/2018_daily_pip_mvmts.xlsx
+++ b/edge_research/2018_daily_pip_mvmts.xlsx
@@ -8,10 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="all_daily_pip_mvmts" sheetId="1" r:id="rId1"/>
-    <sheet name="mvmt -3 pips" sheetId="2" r:id="rId2"/>
-    <sheet name="mvmt -4 pips" sheetId="3" r:id="rId3"/>
-    <sheet name="mvmt -5 pips" sheetId="4" r:id="rId4"/>
-    <sheet name="mvmt -6 pips" sheetId="5" r:id="rId5"/>
+    <sheet name="-3 pips" sheetId="2" r:id="rId2"/>
+    <sheet name="-4 pips" sheetId="3" r:id="rId3"/>
+    <sheet name="-5 pips" sheetId="4" r:id="rId4"/>
+    <sheet name="-6 pips" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>

</xml_diff>